<commit_message>
Changes for go live
</commit_message>
<xml_diff>
--- a/storage/imports/addresses.xlsx
+++ b/storage/imports/addresses.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>address</t>
   </si>
@@ -59,13 +59,64 @@
   </si>
   <si>
     <t>shipping</t>
+  </si>
+  <si>
+    <t>Calle 79B No. 7-60</t>
+  </si>
+  <si>
+    <t>Calle de los anticuarios</t>
+  </si>
+  <si>
+    <t>Daniela Rivera</t>
+  </si>
+  <si>
+    <t>Calle 59 # 8 - 28</t>
+  </si>
+  <si>
+    <t>Chapinero Central</t>
+  </si>
+  <si>
+    <t>John Angel</t>
+  </si>
+  <si>
+    <t>Cra 7 # 45 - 49</t>
+  </si>
+  <si>
+    <t>Carrera 1 #67-21</t>
+  </si>
+  <si>
+    <t>edificio nueva granada etapa1 apto 102</t>
+  </si>
+  <si>
+    <t>Tatiana Luna</t>
+  </si>
+  <si>
+    <t>Calle 10 #11A- 25 sur</t>
+  </si>
+  <si>
+    <t>Ciudad Berna</t>
+  </si>
+  <si>
+    <t>Jennifer Lasprilla</t>
+  </si>
+  <si>
+    <t>Calle 6D # 3-89</t>
+  </si>
+  <si>
+    <t>Candelaria</t>
+  </si>
+  <si>
+    <t>310 854 6364</t>
+  </si>
+  <si>
+    <t>Mercedes Garcia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -76,13 +127,37 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF777777"/>
+      <name val="Oswald"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -100,6 +175,18 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -316,6 +403,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="21.14"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -469,6 +559,234 @@
         <v>3.0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1">
+        <v>110221.0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>524.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3.213723648E9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4.661714</v>
+      </c>
+      <c r="J5" s="1">
+        <v>-74.050852</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="1">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <v>110221.0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>524.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3.022367474E9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4.644743</v>
+      </c>
+      <c r="J6" s="1">
+        <v>-74.062218</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <v>110221.0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>524.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3.12660838E9</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1">
+        <v>4.632111</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-74.06397</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1">
+        <v>110221.0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>524.0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3.108546364E9</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1">
+        <v>4.645672</v>
+      </c>
+      <c r="J8" s="1">
+        <v>-74.051827</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1">
+        <v>110221.0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>524.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3.11524315E9</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1">
+        <v>4.584875</v>
+      </c>
+      <c r="J9" s="1">
+        <v>-74.090762</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1">
+        <v>110221.0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>524.0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="1">
+        <v>4.592404</v>
+      </c>
+      <c r="J10" s="1">
+        <v>-74.074813</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>